<commit_message>
Update Valkyrie Base Frame BOM 00.xlsx
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie Base Frame BOM 00.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie Base Frame BOM 00.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,32 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9A2CC724-BD59-4A97-A172-B6ABF91BF503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:40009_{9A2CC724-BD59-4A97-A172-B6ABF91BF503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A36A5701-D1F7-4DC2-AB21-679B6A6FE84B}"/>
   <bookViews>
-    <workbookView xWindow="34425" yWindow="2925" windowWidth="11640" windowHeight="8460"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valkyrie Base Frame BOM 00" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valkyrie Base Frame BOM 00'!$B$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valkyrie Base Frame BOM 00'!$B$1:$M$13</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Part name</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Length mm</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -118,16 +123,67 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Order Q</t>
-  </si>
-  <si>
     <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Cuts</t>
+  </si>
+  <si>
+    <t>Drop In T Nut</t>
+  </si>
+  <si>
+    <t>M5 Hammer T Nut</t>
+  </si>
+  <si>
+    <t>M5x08 BH</t>
+  </si>
+  <si>
+    <t>BOM Quantity</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>Kit Price</t>
+  </si>
+  <si>
+    <t>Project Valkyrie</t>
+  </si>
+  <si>
+    <t>Total Order Length</t>
+  </si>
+  <si>
+    <t>2040 Total Length</t>
+  </si>
+  <si>
+    <t>2020 Total Length</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>Shop Order Length</t>
+  </si>
+  <si>
+    <t>2040 Order Length</t>
+  </si>
+  <si>
+    <t>Cut Order mm</t>
+  </si>
+  <si>
+    <t>2020 Order Length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,10 +661,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,8 +1023,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -972,222 +1032,538 @@
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <f>J2*H2</f>
+        <v>4</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
-      <c r="G3" s="1">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <f>J3*H3</f>
+        <v>20</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>40</v>
       </c>
-      <c r="G4" s="1">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K4" s="3">
+        <f>J4*H4</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="G5" s="1">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="3">
+        <f>J5*H5</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>40</v>
       </c>
-      <c r="G6" s="1">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="3">
+        <f>J6*H6</f>
+        <v>5</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="K7" s="3">
+        <f>J7*H7</f>
+        <v>11</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>J8*H8</f>
+        <v>6</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
+      <c r="D9">
+        <v>2020</v>
+      </c>
+      <c r="E9">
         <v>500</v>
       </c>
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="G8" s="1">
-        <v>420</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F9">
+        <v>500</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="1"/>
+      <c r="M9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1">
-        <v>460</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="D10">
+        <v>2040</v>
+      </c>
+      <c r="E10">
         <v>500</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>500</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="1"/>
+      <c r="M10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="G11" s="1">
+      <c r="D11">
+        <v>2040</v>
+      </c>
+      <c r="E11">
+        <v>420</v>
+      </c>
+      <c r="F11">
+        <f>E11*C11</f>
+        <v>1680</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>2040</v>
+      </c>
+      <c r="E12">
+        <v>460</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F13" si="0">E12*C12</f>
+        <v>1840</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2040</v>
+      </c>
+      <c r="E13">
         <v>700</v>
       </c>
-      <c r="H11" t="s">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="H13">
         <v>4</v>
       </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4"/>
+      <c r="M13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <f>SUM(I9:I13)</f>
+        <v>11</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <f>J14*I14</f>
+        <v>22</v>
+      </c>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(F10:F14)</f>
+        <v>6820</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2">
+        <f>F9</f>
+        <v>500</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19">
+        <v>1500</v>
+      </c>
+      <c r="J19" s="3">
+        <v>23</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19:K20" si="1">J19*H19</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20">
+        <f>F9</f>
+        <v>500</v>
+      </c>
+      <c r="G20">
+        <v>500</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>6</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="3">
+        <f>SUM(K2:K20)</f>
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H11">
-    <sortCondition ref="B2:B11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:M13">
+    <sortCondition ref="B2:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>